<commit_message>
Added 2 new sites to Weather map
</commit_message>
<xml_diff>
--- a/OmnisharpDatabase01w_addresses.xlsx
+++ b/OmnisharpDatabase01w_addresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Map\OmniLocations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Fluffy Map\OmniMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169ED420-EA08-454C-9CFF-094AA0EA89BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4FF3F8-E6B0-4273-A862-3F0C22D88052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30915" yWindow="1485" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
   </bookViews>
   <sheets>
     <sheet name="PlantData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="151">
   <si>
     <t>Amarillo</t>
   </si>
@@ -465,13 +465,40 @@
   </si>
   <si>
     <t>https://www.gps-coordinates.net/</t>
+  </si>
+  <si>
+    <t>Grand Island</t>
+  </si>
+  <si>
+    <t>Willmar</t>
+  </si>
+  <si>
+    <t>Jennie-O</t>
+  </si>
+  <si>
+    <t>555 South Stuhr Road, Grand Island, NE 68801</t>
+  </si>
+  <si>
+    <t>2505 Willmar Ave SW, Willmar, MN 56201</t>
+  </si>
+  <si>
+    <t>Grand Island', coords</t>
+  </si>
+  <si>
+    <t>Willmar', coords</t>
+  </si>
+  <si>
+    <t>[40.9218949, -98.3205464]</t>
+  </si>
+  <si>
+    <t>[45.1107281, -95.0782776]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,30 +519,6 @@
       <color rgb="FFCCCCCC"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF111111"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -547,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -562,10 +565,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26851CE-C6E3-471D-B829-4B0087AEFA41}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -1115,8 +1115,8 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
+      <c r="E6" s="2">
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>31</v>
@@ -1124,28 +1124,19 @@
       <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
@@ -1157,27 +1148,27 @@
         <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
@@ -1185,51 +1176,51 @@
       <c r="H8" t="s">
         <v>53</v>
       </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
@@ -1238,24 +1229,24 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1267,24 +1258,27 @@
         <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1296,27 +1290,24 @@
         <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -1324,19 +1315,22 @@
       <c r="H13" t="s">
         <v>53</v>
       </c>
+      <c r="L13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -1348,18 +1342,15 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1368,16 +1359,16 @@
         <v>21</v>
       </c>
       <c r="E15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L15" t="s">
         <v>51</v>
@@ -1385,97 +1376,103 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" t="s">
-        <v>53</v>
-      </c>
-      <c r="L17" t="s">
-        <v>52</v>
+        <v>32</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>31</v>
@@ -1483,11 +1480,54 @@
       <c r="G19" t="s">
         <v>27</v>
       </c>
-      <c r="H19" t="s">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L20" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1498,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C220086C-DD4D-400F-8E09-EE751BA6320D}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1555,7 @@
     <col min="10" max="10" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>67</v>
       </c>
@@ -1543,11 +1583,11 @@
       <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>67</v>
       </c>
@@ -1575,11 +1615,11 @@
       <c r="J2" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>67</v>
       </c>
@@ -1607,25 +1647,25 @@
       <c r="J3" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
-        <v>74</v>
+      <c r="B4" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="D4">
-        <v>44.528299500000003</v>
+        <v>40.921894899999998</v>
       </c>
       <c r="E4">
-        <v>-88.090161800000004</v>
+        <v>-98.320546399999998</v>
       </c>
       <c r="G4" t="s">
         <v>98</v>
@@ -1639,25 +1679,25 @@
       <c r="J4" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5">
-        <v>41.55585</v>
+        <v>44.528299500000003</v>
       </c>
       <c r="E5">
-        <v>-90.225245000000001</v>
+        <v>-88.090161800000004</v>
       </c>
       <c r="G5" t="s">
         <v>98</v>
@@ -1671,8 +1711,8 @@
       <c r="J5" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>122</v>
+      <c r="K5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1680,16 +1720,16 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6">
-        <v>40.761811999999999</v>
+        <v>41.55585</v>
       </c>
       <c r="E6">
-        <v>-99.738444000000001</v>
+        <v>-90.225245000000001</v>
       </c>
       <c r="G6" t="s">
         <v>98</v>
@@ -1703,8 +1743,8 @@
       <c r="J6" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>123</v>
+      <c r="K6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1712,16 +1752,16 @@
         <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7">
-        <v>41.209346400000001</v>
+        <v>40.761811999999999</v>
       </c>
       <c r="E7">
-        <v>-95.970134900000005</v>
+        <v>-99.738444000000001</v>
       </c>
       <c r="G7" t="s">
         <v>98</v>
@@ -1735,8 +1775,8 @@
       <c r="J7" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>124</v>
+      <c r="K7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1744,16 +1784,16 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8">
-        <v>46.137530599999998</v>
+        <v>41.209346400000001</v>
       </c>
       <c r="E8">
-        <v>-118.9156132</v>
+        <v>-95.970134900000005</v>
       </c>
       <c r="G8" t="s">
         <v>98</v>
@@ -1767,8 +1807,8 @@
       <c r="J8" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>125</v>
+      <c r="K8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1776,16 +1816,16 @@
         <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9">
-        <v>42.421173600000003</v>
+        <v>46.137530599999998</v>
       </c>
       <c r="E9">
-        <v>-85.649760400000005</v>
+        <v>-118.9156132</v>
       </c>
       <c r="G9" t="s">
         <v>98</v>
@@ -1799,8 +1839,8 @@
       <c r="J9" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>126</v>
+      <c r="K9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1808,16 +1848,16 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10">
-        <v>34.754519100000003</v>
+        <v>42.421173600000003</v>
       </c>
       <c r="E10">
-        <v>-78.807015300000003</v>
+        <v>-85.649760400000005</v>
       </c>
       <c r="G10" t="s">
         <v>98</v>
@@ -1829,10 +1869,10 @@
         <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>127</v>
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1840,16 +1880,16 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11">
-        <v>40.271229599999998</v>
+        <v>34.754519100000003</v>
       </c>
       <c r="E11">
-        <v>-75.336132599999999</v>
+        <v>-78.807015300000003</v>
       </c>
       <c r="G11" t="s">
         <v>98</v>
@@ -1861,10 +1901,10 @@
         <v>70</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="K11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1872,16 +1912,16 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12">
-        <v>42.639209100000002</v>
+        <v>40.271229599999998</v>
       </c>
       <c r="E12">
-        <v>-95.184658099999993</v>
+        <v>-75.336132599999999</v>
       </c>
       <c r="G12" t="s">
         <v>98</v>
@@ -1893,10 +1933,10 @@
         <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>129</v>
+        <v>71</v>
+      </c>
+      <c r="K12" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,16 +1944,16 @@
         <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13">
-        <v>33.441195499999999</v>
+        <v>42.639209100000002</v>
       </c>
       <c r="E13">
-        <v>-112.2553217</v>
+        <v>-95.184658099999993</v>
       </c>
       <c r="G13" t="s">
         <v>98</v>
@@ -1925,10 +1965,10 @@
         <v>70</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>130</v>
+        <v>84</v>
+      </c>
+      <c r="K13" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1936,57 +1976,57 @@
         <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14">
-        <v>30.460480199999999</v>
+        <v>33.441195499999999</v>
       </c>
       <c r="E14">
-        <v>-97.655137100000005</v>
+        <v>-112.2553217</v>
       </c>
       <c r="G14" t="s">
         <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>131</v>
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
-        <v>89</v>
+      <c r="B15" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15">
-        <v>53.472246200000001</v>
-      </c>
-      <c r="E15">
-        <v>-2.3793467000000001</v>
+        <v>150</v>
       </c>
       <c r="G15" t="s">
         <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>91</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>132</v>
+        <v>70</v>
+      </c>
+      <c r="J15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1994,28 +2034,28 @@
         <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16">
-        <v>36.190735099999998</v>
+        <v>30.460480199999999</v>
       </c>
       <c r="E16">
-        <v>-94.474200699999997</v>
+        <v>-97.655137100000005</v>
       </c>
       <c r="G16" t="s">
         <v>98</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I16" t="s">
         <v>88</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>134</v>
+      <c r="K16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2023,31 +2063,28 @@
         <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17">
-        <v>20.9861173</v>
+        <v>53.472246200000001</v>
       </c>
       <c r="E17">
-        <v>-89.793681399999997</v>
+        <v>-2.3793467000000001</v>
       </c>
       <c r="G17" t="s">
         <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2055,31 +2092,28 @@
         <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18">
-        <v>20.674011700000001</v>
+        <v>36.190735099999998</v>
       </c>
       <c r="E18">
-        <v>-103.41797270000001</v>
+        <v>-94.474200699999997</v>
       </c>
       <c r="G18" t="s">
         <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2087,16 +2121,16 @@
         <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D19">
-        <v>25.3220694</v>
+        <v>20.9861173</v>
       </c>
       <c r="E19">
-        <v>-104.908717</v>
+        <v>-89.793681399999997</v>
       </c>
       <c r="G19" t="s">
         <v>98</v>
@@ -2108,48 +2142,112 @@
         <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D20">
-        <v>39.092953399999999</v>
+        <v>20.674011700000001</v>
       </c>
       <c r="E20">
-        <v>-95.643777900000003</v>
+        <v>-103.41797270000001</v>
       </c>
       <c r="G20" t="s">
         <v>98</v>
       </c>
       <c r="H20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21">
+        <v>25.3220694</v>
+      </c>
+      <c r="E21">
+        <v>-104.908717</v>
+      </c>
+      <c r="G21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22">
+        <v>39.092953399999999</v>
+      </c>
+      <c r="E22">
+        <v>-95.643777900000003</v>
+      </c>
+      <c r="G22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" t="s">
         <v>87</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I22" t="s">
         <v>88</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K22" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>